<commit_message>
feat: project cleanup and tracing logic hardening for production
</commit_message>
<xml_diff>
--- a/app/templates/Resumen N-XXX-26 Compresion.xlsx
+++ b/app/templates/Resumen N-XXX-26 Compresion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\crmnew\api-geofal-crm\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019A724B-C414-4B37-9188-7B20AACE51FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455F5966-A16D-41DD-82C2-3B302037BB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <author>HP</author>
   </authors>
   <commentList>
-    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>FORMATO RESUMEN N° F-LEM-P-CO-12.03</t>
+  </si>
+  <si>
+    <t>F'c                             (kg/cm2)</t>
+  </si>
+  <si>
+    <t>Estructura</t>
   </si>
 </sst>
 </file>
@@ -132,7 +138,7 @@
     <numFmt numFmtId="164" formatCode="000\-&quot;CO-26&quot;"/>
     <numFmt numFmtId="165" formatCode="&quot;CERTIFICADO N°&quot;000&quot;-20 AG06&quot;"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +180,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -189,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -282,12 +294,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -355,6 +382,18 @@
     <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -378,13 +417,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>144780</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>274320</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>525628</xdr:rowOff>
@@ -737,19 +776,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="10" width="10.109375" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="11.5546875" style="6"/>
+    <col min="1" max="12" width="10.109375" style="6" customWidth="1"/>
+    <col min="13" max="16384" width="11.5546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15"/>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -759,10 +798,12 @@
       <c r="G1" s="16"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
-      <c r="J1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="17"/>
+    </row>
+    <row r="2" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>24</v>
       </c>
@@ -775,8 +816,10 @@
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
-    </row>
-    <row r="4" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+    </row>
+    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>25</v>
       </c>
@@ -789,281 +832,329 @@
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
-    </row>
-    <row r="5" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+    </row>
+    <row r="5" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="K6" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="K7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I10" s="2" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="I11" s="5" t="s">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="8"/>
+      <c r="K11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="I12" s="5" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="10"/>
+      <c r="K12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I13" s="5" t="s">
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I14" s="5" t="s">
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J14" s="11"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I15" s="5" t="s">
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K15" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="E17" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="F17" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="G17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="H17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="I17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="J17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="K17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="L17" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="21"/>
-    </row>
-    <row r="19" spans="1:10" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="21"/>
+    </row>
+    <row r="19" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="21"/>
-    </row>
-    <row r="20" spans="1:10" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="21"/>
+    </row>
+    <row r="20" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="21"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="21"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="21"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="21"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="21"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="21"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="21"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="21"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="21"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="21"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="21"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="21"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="19"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="21"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="21"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="22"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="21"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="21"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="22"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="21"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="21"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="22"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="21"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="21"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="22"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="19"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="21"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="21"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="22"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="19"/>
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="21"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
chore(tracing): update resumen excel template binary
</commit_message>
<xml_diff>
--- a/app/templates/Resumen N-XXX-26 Compresion.xlsx
+++ b/app/templates/Resumen N-XXX-26 Compresion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\crmnew\api-geofal-crm\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455F5966-A16D-41DD-82C2-3B302037BB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE59AEA2-BFD7-45BD-87A5-C228FB49EB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <author>HP</author>
   </authors>
   <commentList>
-    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="N13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -44,18 +44,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>CLIENTE</t>
   </si>
   <si>
-    <t xml:space="preserve">RECEPCIÓN N° </t>
+    <t>RECEPCIÓN N°</t>
   </si>
   <si>
     <t>DIRECCIÓN **</t>
   </si>
   <si>
-    <t xml:space="preserve">OT N° </t>
+    <t>OT N°</t>
   </si>
   <si>
     <t>PROYECTO **</t>
@@ -67,15 +67,9 @@
     <t>Fecha  Recepción</t>
   </si>
   <si>
-    <t xml:space="preserve">Estructura**     </t>
-  </si>
-  <si>
     <t>Fecha Moldeo**</t>
   </si>
   <si>
-    <t xml:space="preserve">F´c (Kg/cm2) **     </t>
-  </si>
-  <si>
     <t>Fecha Rotura</t>
   </si>
   <si>
@@ -103,7 +97,7 @@
     <t>Longitud                   3</t>
   </si>
   <si>
-    <t xml:space="preserve">Carga                      Máxima            (kN)              </t>
+    <t>Carga                      Máxima            (kN)</t>
   </si>
   <si>
     <t>Tipo                   fractura</t>
@@ -134,11 +128,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="000\-&quot;CO-26&quot;"/>
-    <numFmt numFmtId="165" formatCode="&quot;CERTIFICADO N°&quot;000&quot;-20 AG06&quot;"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;CERTIFICADO N°&quot;000&quot;-20 AG06&quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,19 +157,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <u/>
       <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -201,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -245,26 +228,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -309,12 +272,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -322,12 +337,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -335,19 +344,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -358,42 +354,46 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -418,22 +418,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
+      <xdr:colOff>289560</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
+      <xdr:colOff>495300</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>525628</xdr:rowOff>
+      <xdr:rowOff>502768</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F7822AB-AFFF-4A64-B160-4132E1FCFF3B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04140202-EFD0-4AD2-9EBB-50300C121EF2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -456,7 +456,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2918460" y="60960"/>
+          <a:off x="4373880" y="38100"/>
           <a:ext cx="822960" cy="464668"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -776,36 +776,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="12" width="10.109375" style="6" customWidth="1"/>
-    <col min="13" max="16384" width="11.5546875" style="6"/>
+    <col min="1" max="4" width="10.109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="14" customWidth="1"/>
+    <col min="6" max="8" width="9" style="14" customWidth="1"/>
+    <col min="9" max="16" width="10.109375" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="11.5546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="17"/>
-    </row>
-    <row r="2" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="11"/>
+    </row>
+    <row r="2" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
@@ -818,10 +825,14 @@
       <c r="J3" s="23"/>
       <c r="K3" s="23"/>
       <c r="L3" s="23"/>
-    </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+    </row>
+    <row r="4" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
@@ -834,327 +845,532 @@
       <c r="J4" s="24"/>
       <c r="K4" s="24"/>
       <c r="L4" s="24"/>
-    </row>
-    <row r="5" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+    </row>
+    <row r="5" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="K6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="P6"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="K7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="P7"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="K10" s="2" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11"/>
+    </row>
+    <row r="13" spans="1:16" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="8"/>
-      <c r="K11" s="5" t="s">
+      <c r="F13" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="9"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="10"/>
-      <c r="K12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="K13" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L13" s="11"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="K14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="11"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="K15" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="G13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="J13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="K13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="L13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="M13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="N13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="O13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="P13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="21"/>
-    </row>
-    <row r="19" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="21"/>
-    </row>
-    <row r="20" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="21"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="21"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="21"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="21"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="21"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="21"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="21"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="21"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="21"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="21"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="21"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="21"/>
+    </row>
+    <row r="14" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+    </row>
+    <row r="15" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+    </row>
+    <row r="16" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A35" s="12"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="12"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36" s="18"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="R36" s="12"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B37"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A3:P3"/>
+    <mergeCell ref="A4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>